<commit_message>
Neue Dateien: Logo, Icon, Menu angefangen
</commit_message>
<xml_diff>
--- a/repc_config.xlsx
+++ b/repc_config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patrick\My Drive\05 Python\Python Projekt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23A41C6D-9E5B-4AB3-AAA0-0E2F2950982D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93CBF666-6AB9-47D7-9DB6-1F61148CB63B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9570" yWindow="5505" windowWidth="28830" windowHeight="15360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3510" yWindow="2880" windowWidth="28830" windowHeight="15360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Preisinfo" sheetId="1" r:id="rId1"/>
@@ -623,18 +623,19 @@
   <dimension ref="A1:O17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="22.85546875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="24.140625" bestFit="1" customWidth="1"/>

</xml_diff>